<commit_message>
add genotype to subject metadata
</commit_message>
<xml_diff>
--- a/ephys_nwb_params.xlsx
+++ b/ephys_nwb_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/pac248_pitt_edu/Documents/Thanos Lab Data Management/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pacody/Documents/code/icephys_abf2nwb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{9802FA23-341B-EF40-BBC2-A763867627E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3228CF1-E0C9-BC46-850D-3509CDBDD432}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E65E0B0-3D80-E741-9FEC-6945DB712B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20240" xr2:uid="{163FA3D0-6B63-6049-8518-1A5385667FAD}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20220" xr2:uid="{163FA3D0-6B63-6049-8518-1A5385667FAD}"/>
   </bookViews>
   <sheets>
     <sheet name="EXPERIMENT SESSIONS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>species</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>(YYYYMMDDXXXX)</t>
+  </si>
+  <si>
+    <t>genotype</t>
+  </si>
+  <si>
+    <t>Ntsr1-Cre</t>
   </si>
 </sst>
 </file>
@@ -232,10 +238,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,11 +557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9D9F6C-C3B5-974C-BB35-4505E792027B}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,16 +573,16 @@
     <col min="5" max="5" width="39.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="6.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -603,26 +605,29 @@
         <v>0</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -635,16 +640,16 @@
       <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="K2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="4"/>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2025053001</v>
       </c>
@@ -666,23 +671,26 @@
       <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="L3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2025053001</v>
       </c>
@@ -704,23 +712,26 @@
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -742,19 +753,22 @@
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="J5" s="1">
-        <v>20250531001</v>
       </c>
       <c r="K5" s="1">
         <v>20250531001</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="1">
+        <v>20250531001</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>